<commit_message>
started on inaturalist models
</commit_message>
<xml_diff>
--- a/MODELS.xlsx
+++ b/MODELS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\WYSE\Home\dev\pigallery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D37026E-24D3-49F9-8BDE-E1BA11F41629}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6CB6BB-EC08-43A5-B9B8-10DD54A29316}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{5E1FBCF5-0A35-4073-AF84-4DBDFF6F4B57}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="54">
   <si>
     <t>Model</t>
   </si>
@@ -183,6 +183,21 @@
   </si>
   <si>
     <t>DeepDetect</t>
+  </si>
+  <si>
+    <t>iNaturalist</t>
+  </si>
+  <si>
+    <t>MobileNet v1 Food</t>
+  </si>
+  <si>
+    <t>MobileNet v2 Plants</t>
+  </si>
+  <si>
+    <t>MobileNet v2 Birds</t>
+  </si>
+  <si>
+    <t>MobileNet v2 Insects</t>
   </si>
 </sst>
 </file>
@@ -417,7 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -563,6 +578,12 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
@@ -880,7 +901,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A47E8F53-D3D8-4705-BCEE-FCFF3106DC67}">
-  <dimension ref="B2:X29"/>
+  <dimension ref="B2:X33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2024,6 +2045,162 @@
         <v>34</v>
       </c>
     </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B30" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="36">
+        <v>2023</v>
+      </c>
+      <c r="F30" s="37">
+        <v>20</v>
+      </c>
+      <c r="G30" s="36">
+        <v>58</v>
+      </c>
+      <c r="H30" s="38">
+        <v>192</v>
+      </c>
+      <c r="I30" s="26">
+        <v>45</v>
+      </c>
+      <c r="J30" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="L30" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="M30" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30" s="7"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B31" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="23">
+        <v>2100</v>
+      </c>
+      <c r="F31" s="24">
+        <v>19</v>
+      </c>
+      <c r="G31" s="23">
+        <v>169</v>
+      </c>
+      <c r="H31" s="25">
+        <v>224</v>
+      </c>
+      <c r="I31" s="30">
+        <v>58</v>
+      </c>
+      <c r="J31" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="K31" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="L31" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="M31" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="N31" s="6"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B32" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="23">
+        <v>963</v>
+      </c>
+      <c r="F32" s="24">
+        <v>13</v>
+      </c>
+      <c r="G32" s="23">
+        <v>170</v>
+      </c>
+      <c r="H32" s="25">
+        <v>224</v>
+      </c>
+      <c r="I32" s="30">
+        <v>34</v>
+      </c>
+      <c r="J32" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="L32" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="M32" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="N32" s="6"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B33" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="40">
+        <v>1020</v>
+      </c>
+      <c r="F33" s="41">
+        <v>13</v>
+      </c>
+      <c r="G33" s="40">
+        <v>169</v>
+      </c>
+      <c r="H33" s="42">
+        <v>224</v>
+      </c>
+      <c r="I33" s="43">
+        <v>32</v>
+      </c>
+      <c r="J33" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="K33" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="L33" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="M33" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="N33" s="8"/>
+    </row>
   </sheetData>
   <autoFilter ref="B3:N29" xr:uid="{0041FA21-C734-47E2-9605-B6E4CDD7F534}"/>
   <mergeCells count="1">

</xml_diff>